<commit_message>
modified:   p3.m 	modified:   p3.xlsx 	modified:   parameter.m 	modified:   parameter.mat 	modified:   result3.xlsx
</commit_message>
<xml_diff>
--- a/p3.xlsx
+++ b/p3.xlsx
@@ -60,7 +60,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.08984375" customWidth="true"/>
-    <col min="2" max="2" width="15.08984375" customWidth="true"/>
+    <col min="2" max="2" width="14.453125" customWidth="true"/>
     <col min="3" max="3" width="14.08984375" customWidth="true"/>
     <col min="4" max="4" width="13.453125" customWidth="true"/>
     <col min="5" max="5" width="13.453125" customWidth="true"/>
@@ -85,138 +85,138 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>-0.81712008168391137</v>
+        <v>-0.48954910496300785</v>
       </c>
       <c r="B2" s="0">
-        <v>-1.6384201484689533</v>
+        <v>-0.4946532411966314</v>
       </c>
       <c r="C2" s="0">
-        <v>-1.1548866191425762</v>
+        <v>2.1169021775963999</v>
       </c>
       <c r="D2" s="0">
-        <v>-2.9824586107814897</v>
+        <v>0.24390213106938413</v>
       </c>
       <c r="E2" s="0">
-        <v>-2.780881693504198</v>
+        <v>-4.1168784502176825</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>-0.91918769117663524</v>
+        <v>-0.55158687719685295</v>
       </c>
       <c r="B3" s="0">
-        <v>-1.8295197418143212</v>
+        <v>-0.545685321865641</v>
       </c>
       <c r="C3" s="0">
-        <v>-1.317897616562629</v>
+        <v>2.366408849518074</v>
       </c>
       <c r="D3" s="0">
-        <v>-3.3558158164946077</v>
+        <v>0.30030870120921832</v>
       </c>
       <c r="E3" s="0">
-        <v>-3.1821079143974407</v>
+        <v>-4.675491331345988</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.021000276582185857</v>
+        <v>0.014567646015852356</v>
       </c>
       <c r="B4" s="0">
-        <v>0.026020495845530754</v>
+        <v>0.021094586376653356</v>
       </c>
       <c r="C4" s="0">
-        <v>-0.049755010312173303</v>
+        <v>-0.046004255836585406</v>
       </c>
       <c r="D4" s="0">
-        <v>0.037984933919167983</v>
+        <v>0.035781695249631686</v>
       </c>
       <c r="E4" s="0">
-        <v>0.036847444486705232</v>
+        <v>0.039012422091630805</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.021121137295344584</v>
+        <v>0.014676174674985778</v>
       </c>
       <c r="B5" s="0">
-        <v>0.026463253335853192</v>
+        <v>0.021708004314760592</v>
       </c>
       <c r="C5" s="0">
-        <v>-0.050244377579116498</v>
+        <v>-0.04715666409993139</v>
       </c>
       <c r="D5" s="0">
-        <v>0.038197198597490128</v>
+        <v>0.036465069727266666</v>
       </c>
       <c r="E5" s="0">
-        <v>0.036918650067142782</v>
+        <v>0.039101489229801258</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>1.3392510091063474</v>
+        <v>1.6569998302275373</v>
       </c>
       <c r="B6" s="0">
-        <v>0.50795560850904165</v>
+        <v>1.5461160198025354</v>
       </c>
       <c r="C6" s="0">
-        <v>2.6001656268660462</v>
+        <v>0.75804350810178989</v>
       </c>
       <c r="D6" s="0">
-        <v>4.850001574409216</v>
+        <v>-6.5662890747631133</v>
       </c>
       <c r="E6" s="0">
-        <v>24.014101496256597</v>
+        <v>20.206454679137028</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>1.4733084124466731</v>
+        <v>1.8344092236928842</v>
       </c>
       <c r="B7" s="0">
-        <v>0.56625146973627261</v>
+        <v>1.7433671561146917</v>
       </c>
       <c r="C7" s="0">
-        <v>2.8986021250639986</v>
+        <v>0.85643559192981611</v>
       </c>
       <c r="D7" s="0">
-        <v>5.4480442309808046</v>
+        <v>-7.3624174638324353</v>
       </c>
       <c r="E7" s="0">
-        <v>27.006953681127541</v>
+        <v>22.712249239317536</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>-0.091323768621860354</v>
+        <v>-0.098682227424718591</v>
       </c>
       <c r="B8" s="0">
-        <v>-0.0023216076532560255</v>
+        <v>0.0026991303881585037</v>
       </c>
       <c r="C8" s="0">
-        <v>-0.024927781730624529</v>
+        <v>-0.018205401421277162</v>
       </c>
       <c r="D8" s="0">
-        <v>0.054668443376252249</v>
+        <v>0.041109985583532849</v>
       </c>
       <c r="E8" s="0">
-        <v>0.05324652308464585</v>
+        <v>0.069158423460431911</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>-0.092571613350763915</v>
+        <v>-0.09964626092574011</v>
       </c>
       <c r="B9" s="0">
-        <v>-0.0021031612728150081</v>
+        <v>0.0032214427486452488</v>
       </c>
       <c r="C9" s="0">
-        <v>-0.025710207048688202</v>
+        <v>-0.019360154319327815</v>
       </c>
       <c r="D9" s="0">
-        <v>0.055404344261665045</v>
+        <v>0.040913117377496512</v>
       </c>
       <c r="E9" s="0">
-        <v>0.056114638394941393</v>
+        <v>0.069510524450699732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>